<commit_message>
Deploying to gh-pages from @ GA4GH-Pedigree-Standard/pedigree-fhir-ig@15de6d3d37e5d542f42d80bf7ba4c903d29026c3 🚀
</commit_message>
<xml_diff>
--- a/ValueSet-PedigreeRelationshipTypes.xlsx
+++ b/ValueSet-PedigreeRelationshipTypes.xlsx
@@ -7,7 +7,7 @@
   </bookViews>
   <sheets>
     <sheet name="Metadata" r:id="rId3" sheetId="1"/>
-    <sheet name="Include from kin.fhir" r:id="rId4" sheetId="2"/>
+    <sheet name="Include from Family History R" r:id="rId4" sheetId="2"/>
   </sheets>
 </workbook>
 </file>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2021-10-01T03:36:23+00:00</t>
+    <t>2021-10-11T05:18:50+00:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>